<commit_message>
Automatic update from (popfund)
</commit_message>
<xml_diff>
--- a/IntroStats/Module01/CarStoppingDistances.xlsx
+++ b/IntroStats/Module01/CarStoppingDistances.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aableson\Documents\Webwork\IntroStats\Module01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\aableson\Documents\Webwork\IntroStats\Module01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -345,7 +345,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>